<commit_message>
just an attempt to make morphologic analysis faster
</commit_message>
<xml_diff>
--- a/Nuve/Resources/Tr/suffixes.xlsx
+++ b/Nuve/Resources/Tr/suffixes.xlsx
@@ -2803,9 +2803,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">OZEL_UYOR, DONUSUM_U, </t>
-  </si>
-  <si>
     <t xml:space="preserve">OZEL_GZ, DUSME_UNLU_GZ, DONUSUM_U, DONUSUM_A, </t>
   </si>
   <si>
@@ -2828,6 +2825,9 @@
   </si>
   <si>
     <t xml:space="preserve">DONUSUM_U, YUMUSAMA_kğ, </t>
+  </si>
+  <si>
+    <t>DONUSUM_A, OZEL_OLUMSUZ_UYOR</t>
   </si>
 </sst>
 </file>
@@ -3159,9 +3159,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Ofis Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Ofis">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3199,7 +3199,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Ofis">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -3271,7 +3271,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Ofis">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3448,10 +3448,10 @@
   <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H102" sqref="H102"/>
+      <selection pane="bottomRight" activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5239,7 +5239,7 @@
         <v>396</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>222</v>
@@ -5274,7 +5274,7 @@
         <v>396</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>715</v>
+        <v>630</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>223</v>
@@ -5315,7 +5315,7 @@
         <v>396</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>224</v>
@@ -5753,7 +5753,7 @@
         <v>446</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>222</v>
@@ -5875,7 +5875,7 @@
         <v>446</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>591</v>
@@ -6270,7 +6270,7 @@
         <v>411</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>629</v>
+        <v>723</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>249</v>
@@ -6421,7 +6421,7 @@
         <v>411</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>572</v>
@@ -6453,7 +6453,7 @@
         <v>108</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>604</v>
@@ -6473,7 +6473,7 @@
         <v>108</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>605</v>
@@ -6802,7 +6802,7 @@
         <v>521</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>258</v>
@@ -6834,7 +6834,7 @@
         <v>521</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>613</v>

</xml_diff>